<commit_message>
Get all package versions of a package associated with a process
</commit_message>
<xml_diff>
--- a/Workbooks/EN/Processes.xlsx
+++ b/Workbooks/EN/Processes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Workbooks\EN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F080503B-0210-4DE5-A558-10787162315B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D9F2A15-33D8-4EF8-B478-488383EF2348}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -68,6 +68,12 @@
   </si>
   <si>
     <t>Result</t>
+  </si>
+  <si>
+    <t>Current Package Version</t>
+  </si>
+  <si>
+    <t>All Package Versions</t>
   </si>
 </sst>
 </file>
@@ -292,7 +298,34 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="26">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -975,18 +1008,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table14" displayName="Table14" ref="A1:I201" headerRowDxfId="24" dataDxfId="22" totalsRowDxfId="20" headerRowBorderDxfId="23" tableBorderDxfId="21">
-  <autoFilter ref="A1:I201" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <tableColumns count="9">
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Organization Unit ID" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{058B7C0E-F18D-4AA8-A7A4-2A2B65B79498}" name="Organization Unit Name" dataDxfId="18"/>
-    <tableColumn id="1" xr3:uid="{6FFDE20C-2159-4C8B-AE94-46A18EBF32E7}" name="Process ID" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{81F71C1A-632D-4A5F-BC94-CC97DF7A65EF}" name="Process Name" dataDxfId="16"/>
-    <tableColumn id="9" xr3:uid="{493CAF5E-88C4-4A0A-B010-8B586A753A71}" name="Process Key" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{041C0CE3-E76A-45AF-8F7F-E30A3252DF43}" name="Package Name" dataDxfId="14"/>
-    <tableColumn id="7" xr3:uid="{497F173B-C30A-4F86-8FDC-635553D40209}" name="Package Version" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{F2FC8AF0-A1CD-4EF7-865D-F3BF11667B72}" name="Environment ID" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Environment Name" dataDxfId="11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table14" displayName="Table14" ref="A1:J201" headerRowDxfId="25" dataDxfId="23" totalsRowDxfId="21" headerRowBorderDxfId="24" tableBorderDxfId="22">
+  <autoFilter ref="A1:J201" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <tableColumns count="10">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Organization Unit ID" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{058B7C0E-F18D-4AA8-A7A4-2A2B65B79498}" name="Organization Unit Name" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{6FFDE20C-2159-4C8B-AE94-46A18EBF32E7}" name="Process ID" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{81F71C1A-632D-4A5F-BC94-CC97DF7A65EF}" name="Process Name" dataDxfId="17"/>
+    <tableColumn id="9" xr3:uid="{493CAF5E-88C4-4A0A-B010-8B586A753A71}" name="Process Key" dataDxfId="16"/>
+    <tableColumn id="8" xr3:uid="{041C0CE3-E76A-45AF-8F7F-E30A3252DF43}" name="Package Name" dataDxfId="15"/>
+    <tableColumn id="10" xr3:uid="{28E2D641-5340-4113-9F6E-D4863AB65C09}" name="Current Package Version" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{497F173B-C30A-4F86-8FDC-635553D40209}" name="All Package Versions" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{F2FC8AF0-A1CD-4EF7-865D-F3BF11667B72}" name="Environment ID" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Environment Name" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -996,12 +1030,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F201" totalsRowShown="0">
   <autoFilter ref="A1:F201" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Organization Unit Name" dataDxfId="10"/>
-    <tableColumn id="1" xr3:uid="{E6EA9AC7-5C1D-45D2-A446-988F46C92A27}" name="Environment Name" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Package Name" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{9E1437B9-DDBD-419B-8B2F-273F9FC29E7B}" name="Package Version" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{63649985-044F-4C3A-9B8C-67083E3A106F}" name="Process ID" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{D1E6EAA2-70C4-4033-9FEE-92C367F3E3E4}" name="Result" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Organization Unit Name" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{E6EA9AC7-5C1D-45D2-A446-988F46C92A27}" name="Environment Name" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Package Name" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{9E1437B9-DDBD-419B-8B2F-273F9FC29E7B}" name="Package Version" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{63649985-044F-4C3A-9B8C-67083E3A106F}" name="Process ID" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{D1E6EAA2-70C4-4033-9FEE-92C367F3E3E4}" name="Result" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1011,11 +1045,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A1:E201" totalsRowShown="0">
   <autoFilter ref="A1:E201" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Organization Unit ID" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{282C1FE1-B7D1-4787-943D-6839B4D2A495}" name="Organization Unit Name" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{708D46EC-46F9-46D3-89F1-FC1EA77B5A97}" name="Process ID" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{77482336-B9C3-42EA-B117-2D0B1D764C3A}" name="Process Name" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{9F11D09F-EBB8-481F-9883-602BE1C1BEC7}" name="Result" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Organization Unit ID" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{282C1FE1-B7D1-4787-943D-6839B4D2A495}" name="Organization Unit Name" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{708D46EC-46F9-46D3-89F1-FC1EA77B5A97}" name="Process ID" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{77482336-B9C3-42EA-B117-2D0B1D764C3A}" name="Process Name" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{9F11D09F-EBB8-481F-9883-602BE1C1BEC7}" name="Result" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1284,7 +1318,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2B90804-4CC2-4F3A-A5A0-B313E9BACDDF}">
-  <dimension ref="A1:I201"/>
+  <dimension ref="A1:J201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1298,12 +1332,12 @@
     <col min="4" max="4" width="14.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="36.36328125" style="1" customWidth="1"/>
     <col min="6" max="6" width="15.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.453125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1323,16 +1357,19 @@
         <v>6</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="5"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -1341,9 +1378,10 @@
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
-      <c r="I2" s="7"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I2" s="6"/>
+      <c r="J2" s="7"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="5"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -1352,9 +1390,10 @@
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="7"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I3" s="6"/>
+      <c r="J3" s="7"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="5"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -1363,9 +1402,10 @@
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
-      <c r="I4" s="7"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I4" s="6"/>
+      <c r="J4" s="7"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="5"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -1374,9 +1414,10 @@
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
-      <c r="I5" s="7"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I5" s="6"/>
+      <c r="J5" s="7"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="5"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -1385,9 +1426,10 @@
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
-      <c r="I6" s="7"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I6" s="6"/>
+      <c r="J6" s="7"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="5"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -1396,9 +1438,10 @@
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
-      <c r="I7" s="7"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I7" s="6"/>
+      <c r="J7" s="7"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -1407,9 +1450,10 @@
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
-      <c r="I8" s="7"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I8" s="6"/>
+      <c r="J8" s="7"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="5"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -1418,9 +1462,10 @@
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="7"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I9" s="6"/>
+      <c r="J9" s="7"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="5"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -1429,9 +1474,10 @@
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
-      <c r="I10" s="7"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I10" s="6"/>
+      <c r="J10" s="7"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="8"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
@@ -1440,9 +1486,10 @@
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
-      <c r="I11" s="7"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I11" s="9"/>
+      <c r="J11" s="7"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="8"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
@@ -1451,9 +1498,10 @@
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
-      <c r="I12" s="7"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I12" s="9"/>
+      <c r="J12" s="7"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="8"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
@@ -1462,9 +1510,10 @@
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
-      <c r="I13" s="7"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I13" s="9"/>
+      <c r="J13" s="7"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="8"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
@@ -1473,9 +1522,10 @@
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
-      <c r="I14" s="7"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I14" s="9"/>
+      <c r="J14" s="7"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="8"/>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
@@ -1484,9 +1534,10 @@
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
-      <c r="I15" s="7"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I15" s="9"/>
+      <c r="J15" s="7"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="8"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
@@ -1495,9 +1546,10 @@
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
-      <c r="I16" s="7"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I16" s="9"/>
+      <c r="J16" s="7"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="8"/>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
@@ -1506,9 +1558,10 @@
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
-      <c r="I17" s="7"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I17" s="9"/>
+      <c r="J17" s="7"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="8"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
@@ -1517,9 +1570,10 @@
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
-      <c r="I18" s="7"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I18" s="9"/>
+      <c r="J18" s="7"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="8"/>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
@@ -1528,11 +1582,12 @@
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
       <c r="H19" s="9"/>
-      <c r="I19" s="7" t="s">
+      <c r="I19" s="9"/>
+      <c r="J19" s="7" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="8"/>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
@@ -1541,9 +1596,10 @@
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
       <c r="H20" s="9"/>
-      <c r="I20" s="7"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I20" s="9"/>
+      <c r="J20" s="7"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="8"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
@@ -1552,9 +1608,10 @@
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
-      <c r="I21" s="7"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I21" s="9"/>
+      <c r="J21" s="7"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="8"/>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
@@ -1563,9 +1620,10 @@
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
       <c r="H22" s="9"/>
-      <c r="I22" s="7"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I22" s="9"/>
+      <c r="J22" s="7"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="8"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -1574,9 +1632,10 @@
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
-      <c r="I23" s="7"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I23" s="9"/>
+      <c r="J23" s="7"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="8"/>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
@@ -1585,9 +1644,10 @@
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
-      <c r="I24" s="7"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I24" s="9"/>
+      <c r="J24" s="7"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="8"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
@@ -1596,9 +1656,10 @@
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
-      <c r="I25" s="7"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I25" s="9"/>
+      <c r="J25" s="7"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="8"/>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
@@ -1607,9 +1668,10 @@
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
       <c r="H26" s="9"/>
-      <c r="I26" s="7"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I26" s="9"/>
+      <c r="J26" s="7"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="8"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
@@ -1618,9 +1680,10 @@
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
-      <c r="I27" s="7"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I27" s="9"/>
+      <c r="J27" s="7"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" s="8"/>
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
@@ -1629,9 +1692,10 @@
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
       <c r="H28" s="9"/>
-      <c r="I28" s="7"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I28" s="9"/>
+      <c r="J28" s="7"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" s="8"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
@@ -1640,9 +1704,10 @@
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
-      <c r="I29" s="7"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I29" s="9"/>
+      <c r="J29" s="7"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" s="8"/>
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
@@ -1651,9 +1716,10 @@
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
       <c r="H30" s="9"/>
-      <c r="I30" s="7"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I30" s="9"/>
+      <c r="J30" s="7"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" s="8"/>
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
@@ -1662,9 +1728,10 @@
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
       <c r="H31" s="9"/>
-      <c r="I31" s="7"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I31" s="9"/>
+      <c r="J31" s="7"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" s="8"/>
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
@@ -1673,9 +1740,10 @@
       <c r="F32" s="9"/>
       <c r="G32" s="9"/>
       <c r="H32" s="9"/>
-      <c r="I32" s="7"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I32" s="9"/>
+      <c r="J32" s="7"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="8"/>
       <c r="B33" s="9"/>
       <c r="C33" s="9"/>
@@ -1684,9 +1752,10 @@
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
-      <c r="I33" s="7"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I33" s="9"/>
+      <c r="J33" s="7"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="8"/>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
@@ -1695,9 +1764,10 @@
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
       <c r="H34" s="9"/>
-      <c r="I34" s="7"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I34" s="9"/>
+      <c r="J34" s="7"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" s="8"/>
       <c r="B35" s="9"/>
       <c r="C35" s="9"/>
@@ -1706,9 +1776,10 @@
       <c r="F35" s="9"/>
       <c r="G35" s="9"/>
       <c r="H35" s="9"/>
-      <c r="I35" s="7"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I35" s="9"/>
+      <c r="J35" s="7"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="8"/>
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
@@ -1717,9 +1788,10 @@
       <c r="F36" s="9"/>
       <c r="G36" s="9"/>
       <c r="H36" s="9"/>
-      <c r="I36" s="7"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I36" s="9"/>
+      <c r="J36" s="7"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="8"/>
       <c r="B37" s="9"/>
       <c r="C37" s="9"/>
@@ -1728,9 +1800,10 @@
       <c r="F37" s="9"/>
       <c r="G37" s="9"/>
       <c r="H37" s="9"/>
-      <c r="I37" s="7"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I37" s="9"/>
+      <c r="J37" s="7"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="8"/>
       <c r="B38" s="9"/>
       <c r="C38" s="9"/>
@@ -1739,9 +1812,10 @@
       <c r="F38" s="9"/>
       <c r="G38" s="9"/>
       <c r="H38" s="9"/>
-      <c r="I38" s="7"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I38" s="9"/>
+      <c r="J38" s="7"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" s="8"/>
       <c r="B39" s="9"/>
       <c r="C39" s="9"/>
@@ -1750,9 +1824,10 @@
       <c r="F39" s="9"/>
       <c r="G39" s="9"/>
       <c r="H39" s="9"/>
-      <c r="I39" s="7"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I39" s="9"/>
+      <c r="J39" s="7"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="8"/>
       <c r="B40" s="9"/>
       <c r="C40" s="9"/>
@@ -1761,9 +1836,10 @@
       <c r="F40" s="9"/>
       <c r="G40" s="9"/>
       <c r="H40" s="9"/>
-      <c r="I40" s="7"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I40" s="9"/>
+      <c r="J40" s="7"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" s="8"/>
       <c r="B41" s="9"/>
       <c r="C41" s="9"/>
@@ -1772,9 +1848,10 @@
       <c r="F41" s="9"/>
       <c r="G41" s="9"/>
       <c r="H41" s="9"/>
-      <c r="I41" s="7"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I41" s="9"/>
+      <c r="J41" s="7"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" s="8"/>
       <c r="B42" s="9"/>
       <c r="C42" s="9"/>
@@ -1783,9 +1860,10 @@
       <c r="F42" s="9"/>
       <c r="G42" s="9"/>
       <c r="H42" s="9"/>
-      <c r="I42" s="7"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I42" s="9"/>
+      <c r="J42" s="7"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" s="8"/>
       <c r="B43" s="9"/>
       <c r="C43" s="9"/>
@@ -1794,9 +1872,10 @@
       <c r="F43" s="9"/>
       <c r="G43" s="9"/>
       <c r="H43" s="9"/>
-      <c r="I43" s="7"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I43" s="9"/>
+      <c r="J43" s="7"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" s="8"/>
       <c r="B44" s="9"/>
       <c r="C44" s="9"/>
@@ -1805,9 +1884,10 @@
       <c r="F44" s="9"/>
       <c r="G44" s="9"/>
       <c r="H44" s="9"/>
-      <c r="I44" s="7"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I44" s="9"/>
+      <c r="J44" s="7"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" s="8"/>
       <c r="B45" s="9"/>
       <c r="C45" s="9"/>
@@ -1816,9 +1896,10 @@
       <c r="F45" s="9"/>
       <c r="G45" s="9"/>
       <c r="H45" s="9"/>
-      <c r="I45" s="7"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I45" s="9"/>
+      <c r="J45" s="7"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" s="8"/>
       <c r="B46" s="9"/>
       <c r="C46" s="9"/>
@@ -1827,9 +1908,10 @@
       <c r="F46" s="9"/>
       <c r="G46" s="9"/>
       <c r="H46" s="9"/>
-      <c r="I46" s="7"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I46" s="9"/>
+      <c r="J46" s="7"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" s="8"/>
       <c r="B47" s="9"/>
       <c r="C47" s="9"/>
@@ -1838,9 +1920,10 @@
       <c r="F47" s="9"/>
       <c r="G47" s="9"/>
       <c r="H47" s="9"/>
-      <c r="I47" s="7"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I47" s="9"/>
+      <c r="J47" s="7"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" s="8"/>
       <c r="B48" s="9"/>
       <c r="C48" s="9"/>
@@ -1849,9 +1932,10 @@
       <c r="F48" s="9"/>
       <c r="G48" s="9"/>
       <c r="H48" s="9"/>
-      <c r="I48" s="7"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I48" s="9"/>
+      <c r="J48" s="7"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" s="8"/>
       <c r="B49" s="9"/>
       <c r="C49" s="9"/>
@@ -1860,9 +1944,10 @@
       <c r="F49" s="9"/>
       <c r="G49" s="9"/>
       <c r="H49" s="9"/>
-      <c r="I49" s="7"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I49" s="9"/>
+      <c r="J49" s="7"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50" s="8"/>
       <c r="B50" s="9"/>
       <c r="C50" s="9"/>
@@ -1871,9 +1956,10 @@
       <c r="F50" s="9"/>
       <c r="G50" s="9"/>
       <c r="H50" s="9"/>
-      <c r="I50" s="7"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I50" s="9"/>
+      <c r="J50" s="7"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" s="8"/>
       <c r="B51" s="9"/>
       <c r="C51" s="9"/>
@@ -1882,9 +1968,10 @@
       <c r="F51" s="9"/>
       <c r="G51" s="9"/>
       <c r="H51" s="9"/>
-      <c r="I51" s="7"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I51" s="9"/>
+      <c r="J51" s="7"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52" s="8"/>
       <c r="B52" s="9"/>
       <c r="C52" s="9"/>
@@ -1893,9 +1980,10 @@
       <c r="F52" s="9"/>
       <c r="G52" s="9"/>
       <c r="H52" s="9"/>
-      <c r="I52" s="7"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I52" s="9"/>
+      <c r="J52" s="7"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53" s="8"/>
       <c r="B53" s="9"/>
       <c r="C53" s="9"/>
@@ -1904,9 +1992,10 @@
       <c r="F53" s="9"/>
       <c r="G53" s="9"/>
       <c r="H53" s="9"/>
-      <c r="I53" s="7"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I53" s="9"/>
+      <c r="J53" s="7"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54" s="8"/>
       <c r="B54" s="9"/>
       <c r="C54" s="9"/>
@@ -1915,9 +2004,10 @@
       <c r="F54" s="9"/>
       <c r="G54" s="9"/>
       <c r="H54" s="9"/>
-      <c r="I54" s="7"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I54" s="9"/>
+      <c r="J54" s="7"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55" s="8"/>
       <c r="B55" s="9"/>
       <c r="C55" s="9"/>
@@ -1926,9 +2016,10 @@
       <c r="F55" s="9"/>
       <c r="G55" s="9"/>
       <c r="H55" s="9"/>
-      <c r="I55" s="7"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I55" s="9"/>
+      <c r="J55" s="7"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56" s="8"/>
       <c r="B56" s="9"/>
       <c r="C56" s="9"/>
@@ -1937,9 +2028,10 @@
       <c r="F56" s="9"/>
       <c r="G56" s="9"/>
       <c r="H56" s="9"/>
-      <c r="I56" s="7"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I56" s="9"/>
+      <c r="J56" s="7"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57" s="8"/>
       <c r="B57" s="9"/>
       <c r="C57" s="9"/>
@@ -1948,9 +2040,10 @@
       <c r="F57" s="9"/>
       <c r="G57" s="9"/>
       <c r="H57" s="9"/>
-      <c r="I57" s="7"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I57" s="9"/>
+      <c r="J57" s="7"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58" s="8"/>
       <c r="B58" s="9"/>
       <c r="C58" s="9"/>
@@ -1959,9 +2052,10 @@
       <c r="F58" s="9"/>
       <c r="G58" s="9"/>
       <c r="H58" s="9"/>
-      <c r="I58" s="7"/>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I58" s="9"/>
+      <c r="J58" s="7"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59" s="8"/>
       <c r="B59" s="9"/>
       <c r="C59" s="9"/>
@@ -1970,9 +2064,10 @@
       <c r="F59" s="9"/>
       <c r="G59" s="9"/>
       <c r="H59" s="9"/>
-      <c r="I59" s="7"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I59" s="9"/>
+      <c r="J59" s="7"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60" s="8"/>
       <c r="B60" s="9"/>
       <c r="C60" s="9"/>
@@ -1981,9 +2076,10 @@
       <c r="F60" s="9"/>
       <c r="G60" s="9"/>
       <c r="H60" s="9"/>
-      <c r="I60" s="7"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I60" s="9"/>
+      <c r="J60" s="7"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61" s="8"/>
       <c r="B61" s="9"/>
       <c r="C61" s="9"/>
@@ -1992,9 +2088,10 @@
       <c r="F61" s="9"/>
       <c r="G61" s="9"/>
       <c r="H61" s="9"/>
-      <c r="I61" s="7"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I61" s="9"/>
+      <c r="J61" s="7"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62" s="8"/>
       <c r="B62" s="9"/>
       <c r="C62" s="9"/>
@@ -2003,9 +2100,10 @@
       <c r="F62" s="9"/>
       <c r="G62" s="9"/>
       <c r="H62" s="9"/>
-      <c r="I62" s="7"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I62" s="9"/>
+      <c r="J62" s="7"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63" s="8"/>
       <c r="B63" s="9"/>
       <c r="C63" s="9"/>
@@ -2014,9 +2112,10 @@
       <c r="F63" s="9"/>
       <c r="G63" s="9"/>
       <c r="H63" s="9"/>
-      <c r="I63" s="7"/>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I63" s="9"/>
+      <c r="J63" s="7"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A64" s="8"/>
       <c r="B64" s="9"/>
       <c r="C64" s="9"/>
@@ -2025,9 +2124,10 @@
       <c r="F64" s="9"/>
       <c r="G64" s="9"/>
       <c r="H64" s="9"/>
-      <c r="I64" s="7"/>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I64" s="9"/>
+      <c r="J64" s="7"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65" s="8"/>
       <c r="B65" s="9"/>
       <c r="C65" s="9"/>
@@ -2036,9 +2136,10 @@
       <c r="F65" s="9"/>
       <c r="G65" s="9"/>
       <c r="H65" s="9"/>
-      <c r="I65" s="7"/>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I65" s="9"/>
+      <c r="J65" s="7"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66" s="8"/>
       <c r="B66" s="9"/>
       <c r="C66" s="9"/>
@@ -2047,9 +2148,10 @@
       <c r="F66" s="9"/>
       <c r="G66" s="9"/>
       <c r="H66" s="9"/>
-      <c r="I66" s="7"/>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I66" s="9"/>
+      <c r="J66" s="7"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67" s="8"/>
       <c r="B67" s="9"/>
       <c r="C67" s="9"/>
@@ -2058,9 +2160,10 @@
       <c r="F67" s="9"/>
       <c r="G67" s="9"/>
       <c r="H67" s="9"/>
-      <c r="I67" s="7"/>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I67" s="9"/>
+      <c r="J67" s="7"/>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68" s="8"/>
       <c r="B68" s="9"/>
       <c r="C68" s="9"/>
@@ -2069,9 +2172,10 @@
       <c r="F68" s="9"/>
       <c r="G68" s="9"/>
       <c r="H68" s="9"/>
-      <c r="I68" s="7"/>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I68" s="9"/>
+      <c r="J68" s="7"/>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69" s="8"/>
       <c r="B69" s="9"/>
       <c r="C69" s="9"/>
@@ -2080,9 +2184,10 @@
       <c r="F69" s="9"/>
       <c r="G69" s="9"/>
       <c r="H69" s="9"/>
-      <c r="I69" s="7"/>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I69" s="9"/>
+      <c r="J69" s="7"/>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70" s="8"/>
       <c r="B70" s="9"/>
       <c r="C70" s="9"/>
@@ -2091,9 +2196,10 @@
       <c r="F70" s="9"/>
       <c r="G70" s="9"/>
       <c r="H70" s="9"/>
-      <c r="I70" s="7"/>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I70" s="9"/>
+      <c r="J70" s="7"/>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71" s="8"/>
       <c r="B71" s="9"/>
       <c r="C71" s="9"/>
@@ -2102,9 +2208,10 @@
       <c r="F71" s="9"/>
       <c r="G71" s="9"/>
       <c r="H71" s="9"/>
-      <c r="I71" s="7"/>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I71" s="9"/>
+      <c r="J71" s="7"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72" s="8"/>
       <c r="B72" s="9"/>
       <c r="C72" s="9"/>
@@ -2113,9 +2220,10 @@
       <c r="F72" s="9"/>
       <c r="G72" s="9"/>
       <c r="H72" s="9"/>
-      <c r="I72" s="7"/>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I72" s="9"/>
+      <c r="J72" s="7"/>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73" s="8"/>
       <c r="B73" s="9"/>
       <c r="C73" s="9"/>
@@ -2124,9 +2232,10 @@
       <c r="F73" s="9"/>
       <c r="G73" s="9"/>
       <c r="H73" s="9"/>
-      <c r="I73" s="7"/>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I73" s="9"/>
+      <c r="J73" s="7"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74" s="8"/>
       <c r="B74" s="9"/>
       <c r="C74" s="9"/>
@@ -2135,9 +2244,10 @@
       <c r="F74" s="9"/>
       <c r="G74" s="9"/>
       <c r="H74" s="9"/>
-      <c r="I74" s="7"/>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I74" s="9"/>
+      <c r="J74" s="7"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75" s="8"/>
       <c r="B75" s="9"/>
       <c r="C75" s="9"/>
@@ -2146,9 +2256,10 @@
       <c r="F75" s="9"/>
       <c r="G75" s="9"/>
       <c r="H75" s="9"/>
-      <c r="I75" s="7"/>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I75" s="9"/>
+      <c r="J75" s="7"/>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76" s="8"/>
       <c r="B76" s="9"/>
       <c r="C76" s="9"/>
@@ -2157,9 +2268,10 @@
       <c r="F76" s="9"/>
       <c r="G76" s="9"/>
       <c r="H76" s="9"/>
-      <c r="I76" s="7"/>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I76" s="9"/>
+      <c r="J76" s="7"/>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77" s="8"/>
       <c r="B77" s="9"/>
       <c r="C77" s="9"/>
@@ -2168,9 +2280,10 @@
       <c r="F77" s="9"/>
       <c r="G77" s="9"/>
       <c r="H77" s="9"/>
-      <c r="I77" s="7"/>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I77" s="9"/>
+      <c r="J77" s="7"/>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78" s="8"/>
       <c r="B78" s="9"/>
       <c r="C78" s="9"/>
@@ -2179,9 +2292,10 @@
       <c r="F78" s="9"/>
       <c r="G78" s="9"/>
       <c r="H78" s="9"/>
-      <c r="I78" s="7"/>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I78" s="9"/>
+      <c r="J78" s="7"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A79" s="8"/>
       <c r="B79" s="9"/>
       <c r="C79" s="9"/>
@@ -2190,9 +2304,10 @@
       <c r="F79" s="9"/>
       <c r="G79" s="9"/>
       <c r="H79" s="9"/>
-      <c r="I79" s="7"/>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I79" s="9"/>
+      <c r="J79" s="7"/>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80" s="8"/>
       <c r="B80" s="9"/>
       <c r="C80" s="9"/>
@@ -2201,9 +2316,10 @@
       <c r="F80" s="9"/>
       <c r="G80" s="9"/>
       <c r="H80" s="9"/>
-      <c r="I80" s="7"/>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I80" s="9"/>
+      <c r="J80" s="7"/>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A81" s="8"/>
       <c r="B81" s="9"/>
       <c r="C81" s="9"/>
@@ -2212,9 +2328,10 @@
       <c r="F81" s="9"/>
       <c r="G81" s="9"/>
       <c r="H81" s="9"/>
-      <c r="I81" s="7"/>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I81" s="9"/>
+      <c r="J81" s="7"/>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A82" s="8"/>
       <c r="B82" s="9"/>
       <c r="C82" s="9"/>
@@ -2223,9 +2340,10 @@
       <c r="F82" s="9"/>
       <c r="G82" s="9"/>
       <c r="H82" s="9"/>
-      <c r="I82" s="7"/>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I82" s="9"/>
+      <c r="J82" s="7"/>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83" s="8"/>
       <c r="B83" s="9"/>
       <c r="C83" s="9"/>
@@ -2234,9 +2352,10 @@
       <c r="F83" s="9"/>
       <c r="G83" s="9"/>
       <c r="H83" s="9"/>
-      <c r="I83" s="7"/>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I83" s="9"/>
+      <c r="J83" s="7"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84" s="8"/>
       <c r="B84" s="9"/>
       <c r="C84" s="9"/>
@@ -2245,9 +2364,10 @@
       <c r="F84" s="9"/>
       <c r="G84" s="9"/>
       <c r="H84" s="9"/>
-      <c r="I84" s="7"/>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I84" s="9"/>
+      <c r="J84" s="7"/>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85" s="8"/>
       <c r="B85" s="9"/>
       <c r="C85" s="9"/>
@@ -2256,9 +2376,10 @@
       <c r="F85" s="9"/>
       <c r="G85" s="9"/>
       <c r="H85" s="9"/>
-      <c r="I85" s="7"/>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I85" s="9"/>
+      <c r="J85" s="7"/>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86" s="8"/>
       <c r="B86" s="9"/>
       <c r="C86" s="9"/>
@@ -2267,9 +2388,10 @@
       <c r="F86" s="9"/>
       <c r="G86" s="9"/>
       <c r="H86" s="9"/>
-      <c r="I86" s="7"/>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I86" s="9"/>
+      <c r="J86" s="7"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87" s="8"/>
       <c r="B87" s="9"/>
       <c r="C87" s="9"/>
@@ -2278,9 +2400,10 @@
       <c r="F87" s="9"/>
       <c r="G87" s="9"/>
       <c r="H87" s="9"/>
-      <c r="I87" s="7"/>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I87" s="9"/>
+      <c r="J87" s="7"/>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A88" s="8"/>
       <c r="B88" s="9"/>
       <c r="C88" s="9"/>
@@ -2289,9 +2412,10 @@
       <c r="F88" s="9"/>
       <c r="G88" s="9"/>
       <c r="H88" s="9"/>
-      <c r="I88" s="7"/>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I88" s="9"/>
+      <c r="J88" s="7"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A89" s="8"/>
       <c r="B89" s="9"/>
       <c r="C89" s="9"/>
@@ -2300,9 +2424,10 @@
       <c r="F89" s="9"/>
       <c r="G89" s="9"/>
       <c r="H89" s="9"/>
-      <c r="I89" s="7"/>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I89" s="9"/>
+      <c r="J89" s="7"/>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A90" s="8"/>
       <c r="B90" s="9"/>
       <c r="C90" s="9"/>
@@ -2311,9 +2436,10 @@
       <c r="F90" s="9"/>
       <c r="G90" s="9"/>
       <c r="H90" s="9"/>
-      <c r="I90" s="7"/>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I90" s="9"/>
+      <c r="J90" s="7"/>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A91" s="8"/>
       <c r="B91" s="9"/>
       <c r="C91" s="9"/>
@@ -2322,9 +2448,10 @@
       <c r="F91" s="9"/>
       <c r="G91" s="9"/>
       <c r="H91" s="9"/>
-      <c r="I91" s="7"/>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I91" s="9"/>
+      <c r="J91" s="7"/>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A92" s="8"/>
       <c r="B92" s="9"/>
       <c r="C92" s="9"/>
@@ -2333,9 +2460,10 @@
       <c r="F92" s="9"/>
       <c r="G92" s="9"/>
       <c r="H92" s="9"/>
-      <c r="I92" s="7"/>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I92" s="9"/>
+      <c r="J92" s="7"/>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A93" s="8"/>
       <c r="B93" s="9"/>
       <c r="C93" s="9"/>
@@ -2344,9 +2472,10 @@
       <c r="F93" s="9"/>
       <c r="G93" s="9"/>
       <c r="H93" s="9"/>
-      <c r="I93" s="7"/>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I93" s="9"/>
+      <c r="J93" s="7"/>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A94" s="8"/>
       <c r="B94" s="9"/>
       <c r="C94" s="9"/>
@@ -2355,9 +2484,10 @@
       <c r="F94" s="9"/>
       <c r="G94" s="9"/>
       <c r="H94" s="9"/>
-      <c r="I94" s="7"/>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I94" s="9"/>
+      <c r="J94" s="7"/>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A95" s="8"/>
       <c r="B95" s="9"/>
       <c r="C95" s="9"/>
@@ -2366,9 +2496,10 @@
       <c r="F95" s="9"/>
       <c r="G95" s="9"/>
       <c r="H95" s="9"/>
-      <c r="I95" s="7"/>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I95" s="9"/>
+      <c r="J95" s="7"/>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A96" s="8"/>
       <c r="B96" s="9"/>
       <c r="C96" s="9"/>
@@ -2377,9 +2508,10 @@
       <c r="F96" s="9"/>
       <c r="G96" s="9"/>
       <c r="H96" s="9"/>
-      <c r="I96" s="7"/>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I96" s="9"/>
+      <c r="J96" s="7"/>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A97" s="8"/>
       <c r="B97" s="9"/>
       <c r="C97" s="9"/>
@@ -2388,9 +2520,10 @@
       <c r="F97" s="9"/>
       <c r="G97" s="9"/>
       <c r="H97" s="9"/>
-      <c r="I97" s="7"/>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I97" s="9"/>
+      <c r="J97" s="7"/>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A98" s="8"/>
       <c r="B98" s="9"/>
       <c r="C98" s="9"/>
@@ -2399,9 +2532,10 @@
       <c r="F98" s="9"/>
       <c r="G98" s="9"/>
       <c r="H98" s="9"/>
-      <c r="I98" s="7"/>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I98" s="9"/>
+      <c r="J98" s="7"/>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A99" s="8"/>
       <c r="B99" s="9"/>
       <c r="C99" s="9"/>
@@ -2410,9 +2544,10 @@
       <c r="F99" s="9"/>
       <c r="G99" s="9"/>
       <c r="H99" s="9"/>
-      <c r="I99" s="7"/>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I99" s="9"/>
+      <c r="J99" s="7"/>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A100" s="8"/>
       <c r="B100" s="9"/>
       <c r="C100" s="9"/>
@@ -2421,9 +2556,10 @@
       <c r="F100" s="9"/>
       <c r="G100" s="9"/>
       <c r="H100" s="9"/>
-      <c r="I100" s="7"/>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I100" s="9"/>
+      <c r="J100" s="7"/>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A101" s="8"/>
       <c r="B101" s="9"/>
       <c r="C101" s="9"/>
@@ -2432,9 +2568,10 @@
       <c r="F101" s="9"/>
       <c r="G101" s="9"/>
       <c r="H101" s="9"/>
-      <c r="I101" s="7"/>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I101" s="9"/>
+      <c r="J101" s="7"/>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A102" s="8"/>
       <c r="B102" s="9"/>
       <c r="C102" s="9"/>
@@ -2443,9 +2580,10 @@
       <c r="F102" s="9"/>
       <c r="G102" s="9"/>
       <c r="H102" s="9"/>
-      <c r="I102" s="7"/>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I102" s="9"/>
+      <c r="J102" s="7"/>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A103" s="8"/>
       <c r="B103" s="9"/>
       <c r="C103" s="9"/>
@@ -2454,9 +2592,10 @@
       <c r="F103" s="9"/>
       <c r="G103" s="9"/>
       <c r="H103" s="9"/>
-      <c r="I103" s="7"/>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I103" s="9"/>
+      <c r="J103" s="7"/>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A104" s="8"/>
       <c r="B104" s="9"/>
       <c r="C104" s="9"/>
@@ -2465,9 +2604,10 @@
       <c r="F104" s="9"/>
       <c r="G104" s="9"/>
       <c r="H104" s="9"/>
-      <c r="I104" s="7"/>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I104" s="9"/>
+      <c r="J104" s="7"/>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A105" s="8"/>
       <c r="B105" s="9"/>
       <c r="C105" s="9"/>
@@ -2476,9 +2616,10 @@
       <c r="F105" s="9"/>
       <c r="G105" s="9"/>
       <c r="H105" s="9"/>
-      <c r="I105" s="7"/>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I105" s="9"/>
+      <c r="J105" s="7"/>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A106" s="8"/>
       <c r="B106" s="9"/>
       <c r="C106" s="9"/>
@@ -2487,9 +2628,10 @@
       <c r="F106" s="9"/>
       <c r="G106" s="9"/>
       <c r="H106" s="9"/>
-      <c r="I106" s="7"/>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I106" s="9"/>
+      <c r="J106" s="7"/>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A107" s="8"/>
       <c r="B107" s="9"/>
       <c r="C107" s="9"/>
@@ -2498,9 +2640,10 @@
       <c r="F107" s="9"/>
       <c r="G107" s="9"/>
       <c r="H107" s="9"/>
-      <c r="I107" s="7"/>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I107" s="9"/>
+      <c r="J107" s="7"/>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A108" s="8"/>
       <c r="B108" s="9"/>
       <c r="C108" s="9"/>
@@ -2509,9 +2652,10 @@
       <c r="F108" s="9"/>
       <c r="G108" s="9"/>
       <c r="H108" s="9"/>
-      <c r="I108" s="7"/>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I108" s="9"/>
+      <c r="J108" s="7"/>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A109" s="8"/>
       <c r="B109" s="9"/>
       <c r="C109" s="9"/>
@@ -2520,9 +2664,10 @@
       <c r="F109" s="9"/>
       <c r="G109" s="9"/>
       <c r="H109" s="9"/>
-      <c r="I109" s="7"/>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I109" s="9"/>
+      <c r="J109" s="7"/>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A110" s="8"/>
       <c r="B110" s="9"/>
       <c r="C110" s="9"/>
@@ -2531,9 +2676,10 @@
       <c r="F110" s="9"/>
       <c r="G110" s="9"/>
       <c r="H110" s="9"/>
-      <c r="I110" s="7"/>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I110" s="9"/>
+      <c r="J110" s="7"/>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A111" s="8"/>
       <c r="B111" s="9"/>
       <c r="C111" s="9"/>
@@ -2542,9 +2688,10 @@
       <c r="F111" s="9"/>
       <c r="G111" s="9"/>
       <c r="H111" s="9"/>
-      <c r="I111" s="7"/>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I111" s="9"/>
+      <c r="J111" s="7"/>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A112" s="8"/>
       <c r="B112" s="9"/>
       <c r="C112" s="9"/>
@@ -2553,9 +2700,10 @@
       <c r="F112" s="9"/>
       <c r="G112" s="9"/>
       <c r="H112" s="9"/>
-      <c r="I112" s="7"/>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I112" s="9"/>
+      <c r="J112" s="7"/>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A113" s="8"/>
       <c r="B113" s="9"/>
       <c r="C113" s="9"/>
@@ -2564,9 +2712,10 @@
       <c r="F113" s="9"/>
       <c r="G113" s="9"/>
       <c r="H113" s="9"/>
-      <c r="I113" s="7"/>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I113" s="9"/>
+      <c r="J113" s="7"/>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A114" s="8"/>
       <c r="B114" s="9"/>
       <c r="C114" s="9"/>
@@ -2575,9 +2724,10 @@
       <c r="F114" s="9"/>
       <c r="G114" s="9"/>
       <c r="H114" s="9"/>
-      <c r="I114" s="7"/>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I114" s="9"/>
+      <c r="J114" s="7"/>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A115" s="8"/>
       <c r="B115" s="9"/>
       <c r="C115" s="9"/>
@@ -2586,9 +2736,10 @@
       <c r="F115" s="9"/>
       <c r="G115" s="9"/>
       <c r="H115" s="9"/>
-      <c r="I115" s="7"/>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I115" s="9"/>
+      <c r="J115" s="7"/>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A116" s="8"/>
       <c r="B116" s="9"/>
       <c r="C116" s="9"/>
@@ -2597,9 +2748,10 @@
       <c r="F116" s="9"/>
       <c r="G116" s="9"/>
       <c r="H116" s="9"/>
-      <c r="I116" s="7"/>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I116" s="9"/>
+      <c r="J116" s="7"/>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A117" s="8"/>
       <c r="B117" s="9"/>
       <c r="C117" s="9"/>
@@ -2608,9 +2760,10 @@
       <c r="F117" s="9"/>
       <c r="G117" s="9"/>
       <c r="H117" s="9"/>
-      <c r="I117" s="7"/>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I117" s="9"/>
+      <c r="J117" s="7"/>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A118" s="8"/>
       <c r="B118" s="9"/>
       <c r="C118" s="9"/>
@@ -2619,9 +2772,10 @@
       <c r="F118" s="9"/>
       <c r="G118" s="9"/>
       <c r="H118" s="9"/>
-      <c r="I118" s="7"/>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I118" s="9"/>
+      <c r="J118" s="7"/>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A119" s="8"/>
       <c r="B119" s="9"/>
       <c r="C119" s="9"/>
@@ -2630,9 +2784,10 @@
       <c r="F119" s="9"/>
       <c r="G119" s="9"/>
       <c r="H119" s="9"/>
-      <c r="I119" s="7"/>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I119" s="9"/>
+      <c r="J119" s="7"/>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A120" s="8"/>
       <c r="B120" s="9"/>
       <c r="C120" s="9"/>
@@ -2641,9 +2796,10 @@
       <c r="F120" s="9"/>
       <c r="G120" s="9"/>
       <c r="H120" s="9"/>
-      <c r="I120" s="7"/>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I120" s="9"/>
+      <c r="J120" s="7"/>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A121" s="8"/>
       <c r="B121" s="9"/>
       <c r="C121" s="9"/>
@@ -2652,9 +2808,10 @@
       <c r="F121" s="9"/>
       <c r="G121" s="9"/>
       <c r="H121" s="9"/>
-      <c r="I121" s="7"/>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I121" s="9"/>
+      <c r="J121" s="7"/>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A122" s="8"/>
       <c r="B122" s="9"/>
       <c r="C122" s="9"/>
@@ -2663,9 +2820,10 @@
       <c r="F122" s="9"/>
       <c r="G122" s="9"/>
       <c r="H122" s="9"/>
-      <c r="I122" s="7"/>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I122" s="9"/>
+      <c r="J122" s="7"/>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A123" s="8"/>
       <c r="B123" s="9"/>
       <c r="C123" s="9"/>
@@ -2674,9 +2832,10 @@
       <c r="F123" s="9"/>
       <c r="G123" s="9"/>
       <c r="H123" s="9"/>
-      <c r="I123" s="7"/>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I123" s="9"/>
+      <c r="J123" s="7"/>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A124" s="8"/>
       <c r="B124" s="9"/>
       <c r="C124" s="9"/>
@@ -2685,9 +2844,10 @@
       <c r="F124" s="9"/>
       <c r="G124" s="9"/>
       <c r="H124" s="9"/>
-      <c r="I124" s="7"/>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I124" s="9"/>
+      <c r="J124" s="7"/>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A125" s="8"/>
       <c r="B125" s="9"/>
       <c r="C125" s="9"/>
@@ -2696,9 +2856,10 @@
       <c r="F125" s="9"/>
       <c r="G125" s="9"/>
       <c r="H125" s="9"/>
-      <c r="I125" s="7"/>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I125" s="9"/>
+      <c r="J125" s="7"/>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A126" s="8"/>
       <c r="B126" s="9"/>
       <c r="C126" s="9"/>
@@ -2707,9 +2868,10 @@
       <c r="F126" s="9"/>
       <c r="G126" s="9"/>
       <c r="H126" s="9"/>
-      <c r="I126" s="7"/>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I126" s="9"/>
+      <c r="J126" s="7"/>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A127" s="8"/>
       <c r="B127" s="9"/>
       <c r="C127" s="9"/>
@@ -2718,9 +2880,10 @@
       <c r="F127" s="9"/>
       <c r="G127" s="9"/>
       <c r="H127" s="9"/>
-      <c r="I127" s="7"/>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I127" s="9"/>
+      <c r="J127" s="7"/>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A128" s="8"/>
       <c r="B128" s="9"/>
       <c r="C128" s="9"/>
@@ -2729,9 +2892,10 @@
       <c r="F128" s="9"/>
       <c r="G128" s="9"/>
       <c r="H128" s="9"/>
-      <c r="I128" s="7"/>
-    </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I128" s="9"/>
+      <c r="J128" s="7"/>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A129" s="8"/>
       <c r="B129" s="9"/>
       <c r="C129" s="9"/>
@@ -2740,9 +2904,10 @@
       <c r="F129" s="9"/>
       <c r="G129" s="9"/>
       <c r="H129" s="9"/>
-      <c r="I129" s="7"/>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I129" s="9"/>
+      <c r="J129" s="7"/>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A130" s="8"/>
       <c r="B130" s="9"/>
       <c r="C130" s="9"/>
@@ -2751,9 +2916,10 @@
       <c r="F130" s="9"/>
       <c r="G130" s="9"/>
       <c r="H130" s="9"/>
-      <c r="I130" s="7"/>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I130" s="9"/>
+      <c r="J130" s="7"/>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A131" s="8"/>
       <c r="B131" s="9"/>
       <c r="C131" s="9"/>
@@ -2762,9 +2928,10 @@
       <c r="F131" s="9"/>
       <c r="G131" s="9"/>
       <c r="H131" s="9"/>
-      <c r="I131" s="7"/>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I131" s="9"/>
+      <c r="J131" s="7"/>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A132" s="8"/>
       <c r="B132" s="9"/>
       <c r="C132" s="9"/>
@@ -2773,9 +2940,10 @@
       <c r="F132" s="9"/>
       <c r="G132" s="9"/>
       <c r="H132" s="9"/>
-      <c r="I132" s="7"/>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I132" s="9"/>
+      <c r="J132" s="7"/>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A133" s="8"/>
       <c r="B133" s="9"/>
       <c r="C133" s="9"/>
@@ -2784,9 +2952,10 @@
       <c r="F133" s="9"/>
       <c r="G133" s="9"/>
       <c r="H133" s="9"/>
-      <c r="I133" s="7"/>
-    </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I133" s="9"/>
+      <c r="J133" s="7"/>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A134" s="8"/>
       <c r="B134" s="9"/>
       <c r="C134" s="9"/>
@@ -2795,9 +2964,10 @@
       <c r="F134" s="9"/>
       <c r="G134" s="9"/>
       <c r="H134" s="9"/>
-      <c r="I134" s="7"/>
-    </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I134" s="9"/>
+      <c r="J134" s="7"/>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A135" s="8"/>
       <c r="B135" s="9"/>
       <c r="C135" s="9"/>
@@ -2806,9 +2976,10 @@
       <c r="F135" s="9"/>
       <c r="G135" s="9"/>
       <c r="H135" s="9"/>
-      <c r="I135" s="7"/>
-    </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I135" s="9"/>
+      <c r="J135" s="7"/>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A136" s="8"/>
       <c r="B136" s="9"/>
       <c r="C136" s="9"/>
@@ -2817,9 +2988,10 @@
       <c r="F136" s="9"/>
       <c r="G136" s="9"/>
       <c r="H136" s="9"/>
-      <c r="I136" s="7"/>
-    </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I136" s="9"/>
+      <c r="J136" s="7"/>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A137" s="8"/>
       <c r="B137" s="9"/>
       <c r="C137" s="9"/>
@@ -2828,9 +3000,10 @@
       <c r="F137" s="9"/>
       <c r="G137" s="9"/>
       <c r="H137" s="9"/>
-      <c r="I137" s="7"/>
-    </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I137" s="9"/>
+      <c r="J137" s="7"/>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A138" s="8"/>
       <c r="B138" s="9"/>
       <c r="C138" s="9"/>
@@ -2839,9 +3012,10 @@
       <c r="F138" s="9"/>
       <c r="G138" s="9"/>
       <c r="H138" s="9"/>
-      <c r="I138" s="7"/>
-    </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I138" s="9"/>
+      <c r="J138" s="7"/>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A139" s="8"/>
       <c r="B139" s="9"/>
       <c r="C139" s="9"/>
@@ -2850,9 +3024,10 @@
       <c r="F139" s="9"/>
       <c r="G139" s="9"/>
       <c r="H139" s="9"/>
-      <c r="I139" s="7"/>
-    </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I139" s="9"/>
+      <c r="J139" s="7"/>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A140" s="8"/>
       <c r="B140" s="9"/>
       <c r="C140" s="9"/>
@@ -2861,9 +3036,10 @@
       <c r="F140" s="9"/>
       <c r="G140" s="9"/>
       <c r="H140" s="9"/>
-      <c r="I140" s="7"/>
-    </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I140" s="9"/>
+      <c r="J140" s="7"/>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A141" s="8"/>
       <c r="B141" s="9"/>
       <c r="C141" s="9"/>
@@ -2872,9 +3048,10 @@
       <c r="F141" s="9"/>
       <c r="G141" s="9"/>
       <c r="H141" s="9"/>
-      <c r="I141" s="7"/>
-    </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I141" s="9"/>
+      <c r="J141" s="7"/>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A142" s="8"/>
       <c r="B142" s="9"/>
       <c r="C142" s="9"/>
@@ -2883,9 +3060,10 @@
       <c r="F142" s="9"/>
       <c r="G142" s="9"/>
       <c r="H142" s="9"/>
-      <c r="I142" s="7"/>
-    </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I142" s="9"/>
+      <c r="J142" s="7"/>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A143" s="8"/>
       <c r="B143" s="9"/>
       <c r="C143" s="9"/>
@@ -2894,9 +3072,10 @@
       <c r="F143" s="9"/>
       <c r="G143" s="9"/>
       <c r="H143" s="9"/>
-      <c r="I143" s="7"/>
-    </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I143" s="9"/>
+      <c r="J143" s="7"/>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A144" s="8"/>
       <c r="B144" s="9"/>
       <c r="C144" s="9"/>
@@ -2905,9 +3084,10 @@
       <c r="F144" s="9"/>
       <c r="G144" s="9"/>
       <c r="H144" s="9"/>
-      <c r="I144" s="7"/>
-    </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I144" s="9"/>
+      <c r="J144" s="7"/>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A145" s="8"/>
       <c r="B145" s="9"/>
       <c r="C145" s="9"/>
@@ -2916,9 +3096,10 @@
       <c r="F145" s="9"/>
       <c r="G145" s="9"/>
       <c r="H145" s="9"/>
-      <c r="I145" s="7"/>
-    </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I145" s="9"/>
+      <c r="J145" s="7"/>
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A146" s="8"/>
       <c r="B146" s="9"/>
       <c r="C146" s="9"/>
@@ -2927,9 +3108,10 @@
       <c r="F146" s="9"/>
       <c r="G146" s="9"/>
       <c r="H146" s="9"/>
-      <c r="I146" s="7"/>
-    </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I146" s="9"/>
+      <c r="J146" s="7"/>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A147" s="8"/>
       <c r="B147" s="9"/>
       <c r="C147" s="9"/>
@@ -2938,9 +3120,10 @@
       <c r="F147" s="9"/>
       <c r="G147" s="9"/>
       <c r="H147" s="9"/>
-      <c r="I147" s="7"/>
-    </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I147" s="9"/>
+      <c r="J147" s="7"/>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A148" s="8"/>
       <c r="B148" s="9"/>
       <c r="C148" s="9"/>
@@ -2949,9 +3132,10 @@
       <c r="F148" s="9"/>
       <c r="G148" s="9"/>
       <c r="H148" s="9"/>
-      <c r="I148" s="7"/>
-    </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I148" s="9"/>
+      <c r="J148" s="7"/>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A149" s="8"/>
       <c r="B149" s="9"/>
       <c r="C149" s="9"/>
@@ -2960,9 +3144,10 @@
       <c r="F149" s="9"/>
       <c r="G149" s="9"/>
       <c r="H149" s="9"/>
-      <c r="I149" s="7"/>
-    </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I149" s="9"/>
+      <c r="J149" s="7"/>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A150" s="8"/>
       <c r="B150" s="9"/>
       <c r="C150" s="9"/>
@@ -2971,9 +3156,10 @@
       <c r="F150" s="9"/>
       <c r="G150" s="9"/>
       <c r="H150" s="9"/>
-      <c r="I150" s="7"/>
-    </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I150" s="9"/>
+      <c r="J150" s="7"/>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A151" s="8"/>
       <c r="B151" s="9"/>
       <c r="C151" s="9"/>
@@ -2982,9 +3168,10 @@
       <c r="F151" s="9"/>
       <c r="G151" s="9"/>
       <c r="H151" s="9"/>
-      <c r="I151" s="7"/>
-    </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I151" s="9"/>
+      <c r="J151" s="7"/>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A152" s="8"/>
       <c r="B152" s="9"/>
       <c r="C152" s="9"/>
@@ -2993,9 +3180,10 @@
       <c r="F152" s="9"/>
       <c r="G152" s="9"/>
       <c r="H152" s="9"/>
-      <c r="I152" s="7"/>
-    </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I152" s="9"/>
+      <c r="J152" s="7"/>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A153" s="8"/>
       <c r="B153" s="9"/>
       <c r="C153" s="9"/>
@@ -3004,9 +3192,10 @@
       <c r="F153" s="9"/>
       <c r="G153" s="9"/>
       <c r="H153" s="9"/>
-      <c r="I153" s="7"/>
-    </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I153" s="9"/>
+      <c r="J153" s="7"/>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A154" s="8"/>
       <c r="B154" s="9"/>
       <c r="C154" s="9"/>
@@ -3015,9 +3204,10 @@
       <c r="F154" s="9"/>
       <c r="G154" s="9"/>
       <c r="H154" s="9"/>
-      <c r="I154" s="7"/>
-    </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I154" s="9"/>
+      <c r="J154" s="7"/>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A155" s="8"/>
       <c r="B155" s="9"/>
       <c r="C155" s="9"/>
@@ -3026,9 +3216,10 @@
       <c r="F155" s="9"/>
       <c r="G155" s="9"/>
       <c r="H155" s="9"/>
-      <c r="I155" s="7"/>
-    </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I155" s="9"/>
+      <c r="J155" s="7"/>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A156" s="8"/>
       <c r="B156" s="9"/>
       <c r="C156" s="9"/>
@@ -3037,9 +3228,10 @@
       <c r="F156" s="9"/>
       <c r="G156" s="9"/>
       <c r="H156" s="9"/>
-      <c r="I156" s="7"/>
-    </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I156" s="9"/>
+      <c r="J156" s="7"/>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A157" s="8"/>
       <c r="B157" s="9"/>
       <c r="C157" s="9"/>
@@ -3048,9 +3240,10 @@
       <c r="F157" s="9"/>
       <c r="G157" s="9"/>
       <c r="H157" s="9"/>
-      <c r="I157" s="7"/>
-    </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I157" s="9"/>
+      <c r="J157" s="7"/>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A158" s="8"/>
       <c r="B158" s="9"/>
       <c r="C158" s="9"/>
@@ -3059,9 +3252,10 @@
       <c r="F158" s="9"/>
       <c r="G158" s="9"/>
       <c r="H158" s="9"/>
-      <c r="I158" s="7"/>
-    </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I158" s="9"/>
+      <c r="J158" s="7"/>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A159" s="8"/>
       <c r="B159" s="9"/>
       <c r="C159" s="9"/>
@@ -3070,9 +3264,10 @@
       <c r="F159" s="9"/>
       <c r="G159" s="9"/>
       <c r="H159" s="9"/>
-      <c r="I159" s="7"/>
-    </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I159" s="9"/>
+      <c r="J159" s="7"/>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A160" s="8"/>
       <c r="B160" s="9"/>
       <c r="C160" s="9"/>
@@ -3081,9 +3276,10 @@
       <c r="F160" s="9"/>
       <c r="G160" s="9"/>
       <c r="H160" s="9"/>
-      <c r="I160" s="7"/>
-    </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I160" s="9"/>
+      <c r="J160" s="7"/>
+    </row>
+    <row r="161" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A161" s="8"/>
       <c r="B161" s="9"/>
       <c r="C161" s="9"/>
@@ -3092,9 +3288,10 @@
       <c r="F161" s="9"/>
       <c r="G161" s="9"/>
       <c r="H161" s="9"/>
-      <c r="I161" s="7"/>
-    </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I161" s="9"/>
+      <c r="J161" s="7"/>
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A162" s="8"/>
       <c r="B162" s="9"/>
       <c r="C162" s="9"/>
@@ -3103,9 +3300,10 @@
       <c r="F162" s="9"/>
       <c r="G162" s="9"/>
       <c r="H162" s="9"/>
-      <c r="I162" s="7"/>
-    </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I162" s="9"/>
+      <c r="J162" s="7"/>
+    </row>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A163" s="8"/>
       <c r="B163" s="9"/>
       <c r="C163" s="9"/>
@@ -3114,9 +3312,10 @@
       <c r="F163" s="9"/>
       <c r="G163" s="9"/>
       <c r="H163" s="9"/>
-      <c r="I163" s="7"/>
-    </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I163" s="9"/>
+      <c r="J163" s="7"/>
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A164" s="8"/>
       <c r="B164" s="9"/>
       <c r="C164" s="9"/>
@@ -3125,9 +3324,10 @@
       <c r="F164" s="9"/>
       <c r="G164" s="9"/>
       <c r="H164" s="9"/>
-      <c r="I164" s="7"/>
-    </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I164" s="9"/>
+      <c r="J164" s="7"/>
+    </row>
+    <row r="165" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A165" s="8"/>
       <c r="B165" s="9"/>
       <c r="C165" s="9"/>
@@ -3136,9 +3336,10 @@
       <c r="F165" s="9"/>
       <c r="G165" s="9"/>
       <c r="H165" s="9"/>
-      <c r="I165" s="7"/>
-    </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I165" s="9"/>
+      <c r="J165" s="7"/>
+    </row>
+    <row r="166" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A166" s="8"/>
       <c r="B166" s="9"/>
       <c r="C166" s="9"/>
@@ -3147,9 +3348,10 @@
       <c r="F166" s="9"/>
       <c r="G166" s="9"/>
       <c r="H166" s="9"/>
-      <c r="I166" s="7"/>
-    </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I166" s="9"/>
+      <c r="J166" s="7"/>
+    </row>
+    <row r="167" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A167" s="8"/>
       <c r="B167" s="9"/>
       <c r="C167" s="9"/>
@@ -3158,9 +3360,10 @@
       <c r="F167" s="9"/>
       <c r="G167" s="9"/>
       <c r="H167" s="9"/>
-      <c r="I167" s="7"/>
-    </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I167" s="9"/>
+      <c r="J167" s="7"/>
+    </row>
+    <row r="168" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A168" s="8"/>
       <c r="B168" s="9"/>
       <c r="C168" s="9"/>
@@ -3169,9 +3372,10 @@
       <c r="F168" s="9"/>
       <c r="G168" s="9"/>
       <c r="H168" s="9"/>
-      <c r="I168" s="7"/>
-    </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I168" s="9"/>
+      <c r="J168" s="7"/>
+    </row>
+    <row r="169" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A169" s="8"/>
       <c r="B169" s="9"/>
       <c r="C169" s="9"/>
@@ -3180,9 +3384,10 @@
       <c r="F169" s="9"/>
       <c r="G169" s="9"/>
       <c r="H169" s="9"/>
-      <c r="I169" s="7"/>
-    </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I169" s="9"/>
+      <c r="J169" s="7"/>
+    </row>
+    <row r="170" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A170" s="8"/>
       <c r="B170" s="9"/>
       <c r="C170" s="9"/>
@@ -3191,9 +3396,10 @@
       <c r="F170" s="9"/>
       <c r="G170" s="9"/>
       <c r="H170" s="9"/>
-      <c r="I170" s="7"/>
-    </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I170" s="9"/>
+      <c r="J170" s="7"/>
+    </row>
+    <row r="171" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A171" s="8"/>
       <c r="B171" s="9"/>
       <c r="C171" s="9"/>
@@ -3202,9 +3408,10 @@
       <c r="F171" s="9"/>
       <c r="G171" s="9"/>
       <c r="H171" s="9"/>
-      <c r="I171" s="7"/>
-    </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I171" s="9"/>
+      <c r="J171" s="7"/>
+    </row>
+    <row r="172" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A172" s="8"/>
       <c r="B172" s="9"/>
       <c r="C172" s="9"/>
@@ -3213,9 +3420,10 @@
       <c r="F172" s="9"/>
       <c r="G172" s="9"/>
       <c r="H172" s="9"/>
-      <c r="I172" s="7"/>
-    </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I172" s="9"/>
+      <c r="J172" s="7"/>
+    </row>
+    <row r="173" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A173" s="8"/>
       <c r="B173" s="9"/>
       <c r="C173" s="9"/>
@@ -3224,9 +3432,10 @@
       <c r="F173" s="9"/>
       <c r="G173" s="9"/>
       <c r="H173" s="9"/>
-      <c r="I173" s="7"/>
-    </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I173" s="9"/>
+      <c r="J173" s="7"/>
+    </row>
+    <row r="174" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A174" s="8"/>
       <c r="B174" s="9"/>
       <c r="C174" s="9"/>
@@ -3235,9 +3444,10 @@
       <c r="F174" s="9"/>
       <c r="G174" s="9"/>
       <c r="H174" s="9"/>
-      <c r="I174" s="7"/>
-    </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I174" s="9"/>
+      <c r="J174" s="7"/>
+    </row>
+    <row r="175" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A175" s="8"/>
       <c r="B175" s="9"/>
       <c r="C175" s="9"/>
@@ -3246,9 +3456,10 @@
       <c r="F175" s="9"/>
       <c r="G175" s="9"/>
       <c r="H175" s="9"/>
-      <c r="I175" s="7"/>
-    </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I175" s="9"/>
+      <c r="J175" s="7"/>
+    </row>
+    <row r="176" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A176" s="8"/>
       <c r="B176" s="9"/>
       <c r="C176" s="9"/>
@@ -3257,9 +3468,10 @@
       <c r="F176" s="9"/>
       <c r="G176" s="9"/>
       <c r="H176" s="9"/>
-      <c r="I176" s="7"/>
-    </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I176" s="9"/>
+      <c r="J176" s="7"/>
+    </row>
+    <row r="177" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A177" s="8"/>
       <c r="B177" s="9"/>
       <c r="C177" s="9"/>
@@ -3268,9 +3480,10 @@
       <c r="F177" s="9"/>
       <c r="G177" s="9"/>
       <c r="H177" s="9"/>
-      <c r="I177" s="7"/>
-    </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I177" s="9"/>
+      <c r="J177" s="7"/>
+    </row>
+    <row r="178" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A178" s="8"/>
       <c r="B178" s="9"/>
       <c r="C178" s="9"/>
@@ -3279,9 +3492,10 @@
       <c r="F178" s="9"/>
       <c r="G178" s="9"/>
       <c r="H178" s="9"/>
-      <c r="I178" s="7"/>
-    </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I178" s="9"/>
+      <c r="J178" s="7"/>
+    </row>
+    <row r="179" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A179" s="8"/>
       <c r="B179" s="9"/>
       <c r="C179" s="9"/>
@@ -3290,9 +3504,10 @@
       <c r="F179" s="9"/>
       <c r="G179" s="9"/>
       <c r="H179" s="9"/>
-      <c r="I179" s="7"/>
-    </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I179" s="9"/>
+      <c r="J179" s="7"/>
+    </row>
+    <row r="180" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A180" s="8"/>
       <c r="B180" s="9"/>
       <c r="C180" s="9"/>
@@ -3301,9 +3516,10 @@
       <c r="F180" s="9"/>
       <c r="G180" s="9"/>
       <c r="H180" s="9"/>
-      <c r="I180" s="7"/>
-    </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I180" s="9"/>
+      <c r="J180" s="7"/>
+    </row>
+    <row r="181" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A181" s="8"/>
       <c r="B181" s="9"/>
       <c r="C181" s="9"/>
@@ -3312,9 +3528,10 @@
       <c r="F181" s="9"/>
       <c r="G181" s="9"/>
       <c r="H181" s="9"/>
-      <c r="I181" s="7"/>
-    </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I181" s="9"/>
+      <c r="J181" s="7"/>
+    </row>
+    <row r="182" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A182" s="8"/>
       <c r="B182" s="9"/>
       <c r="C182" s="9"/>
@@ -3323,9 +3540,10 @@
       <c r="F182" s="9"/>
       <c r="G182" s="9"/>
       <c r="H182" s="9"/>
-      <c r="I182" s="7"/>
-    </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I182" s="9"/>
+      <c r="J182" s="7"/>
+    </row>
+    <row r="183" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A183" s="8"/>
       <c r="B183" s="9"/>
       <c r="C183" s="9"/>
@@ -3334,9 +3552,10 @@
       <c r="F183" s="9"/>
       <c r="G183" s="9"/>
       <c r="H183" s="9"/>
-      <c r="I183" s="7"/>
-    </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I183" s="9"/>
+      <c r="J183" s="7"/>
+    </row>
+    <row r="184" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A184" s="8"/>
       <c r="B184" s="9"/>
       <c r="C184" s="9"/>
@@ -3345,9 +3564,10 @@
       <c r="F184" s="9"/>
       <c r="G184" s="9"/>
       <c r="H184" s="9"/>
-      <c r="I184" s="7"/>
-    </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I184" s="9"/>
+      <c r="J184" s="7"/>
+    </row>
+    <row r="185" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A185" s="8"/>
       <c r="B185" s="9"/>
       <c r="C185" s="9"/>
@@ -3356,9 +3576,10 @@
       <c r="F185" s="9"/>
       <c r="G185" s="9"/>
       <c r="H185" s="9"/>
-      <c r="I185" s="7"/>
-    </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I185" s="9"/>
+      <c r="J185" s="7"/>
+    </row>
+    <row r="186" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A186" s="8"/>
       <c r="B186" s="9"/>
       <c r="C186" s="9"/>
@@ -3367,9 +3588,10 @@
       <c r="F186" s="9"/>
       <c r="G186" s="9"/>
       <c r="H186" s="9"/>
-      <c r="I186" s="7"/>
-    </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I186" s="9"/>
+      <c r="J186" s="7"/>
+    </row>
+    <row r="187" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A187" s="8"/>
       <c r="B187" s="9"/>
       <c r="C187" s="9"/>
@@ -3378,9 +3600,10 @@
       <c r="F187" s="9"/>
       <c r="G187" s="9"/>
       <c r="H187" s="9"/>
-      <c r="I187" s="7"/>
-    </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I187" s="9"/>
+      <c r="J187" s="7"/>
+    </row>
+    <row r="188" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A188" s="8"/>
       <c r="B188" s="9"/>
       <c r="C188" s="9"/>
@@ -3389,9 +3612,10 @@
       <c r="F188" s="9"/>
       <c r="G188" s="9"/>
       <c r="H188" s="9"/>
-      <c r="I188" s="7"/>
-    </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I188" s="9"/>
+      <c r="J188" s="7"/>
+    </row>
+    <row r="189" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A189" s="8"/>
       <c r="B189" s="9"/>
       <c r="C189" s="9"/>
@@ -3400,9 +3624,10 @@
       <c r="F189" s="9"/>
       <c r="G189" s="9"/>
       <c r="H189" s="9"/>
-      <c r="I189" s="7"/>
-    </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I189" s="9"/>
+      <c r="J189" s="7"/>
+    </row>
+    <row r="190" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A190" s="8"/>
       <c r="B190" s="9"/>
       <c r="C190" s="9"/>
@@ -3411,9 +3636,10 @@
       <c r="F190" s="9"/>
       <c r="G190" s="9"/>
       <c r="H190" s="9"/>
-      <c r="I190" s="7"/>
-    </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I190" s="9"/>
+      <c r="J190" s="7"/>
+    </row>
+    <row r="191" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A191" s="8"/>
       <c r="B191" s="9"/>
       <c r="C191" s="9"/>
@@ -3422,9 +3648,10 @@
       <c r="F191" s="9"/>
       <c r="G191" s="9"/>
       <c r="H191" s="9"/>
-      <c r="I191" s="7"/>
-    </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I191" s="9"/>
+      <c r="J191" s="7"/>
+    </row>
+    <row r="192" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A192" s="8"/>
       <c r="B192" s="9"/>
       <c r="C192" s="9"/>
@@ -3433,9 +3660,10 @@
       <c r="F192" s="9"/>
       <c r="G192" s="9"/>
       <c r="H192" s="9"/>
-      <c r="I192" s="7"/>
-    </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I192" s="9"/>
+      <c r="J192" s="7"/>
+    </row>
+    <row r="193" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A193" s="8"/>
       <c r="B193" s="9"/>
       <c r="C193" s="9"/>
@@ -3444,9 +3672,10 @@
       <c r="F193" s="9"/>
       <c r="G193" s="9"/>
       <c r="H193" s="9"/>
-      <c r="I193" s="7"/>
-    </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I193" s="9"/>
+      <c r="J193" s="7"/>
+    </row>
+    <row r="194" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A194" s="8"/>
       <c r="B194" s="9"/>
       <c r="C194" s="9"/>
@@ -3455,9 +3684,10 @@
       <c r="F194" s="9"/>
       <c r="G194" s="9"/>
       <c r="H194" s="9"/>
-      <c r="I194" s="7"/>
-    </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I194" s="9"/>
+      <c r="J194" s="7"/>
+    </row>
+    <row r="195" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A195" s="8"/>
       <c r="B195" s="9"/>
       <c r="C195" s="9"/>
@@ -3466,9 +3696,10 @@
       <c r="F195" s="9"/>
       <c r="G195" s="9"/>
       <c r="H195" s="9"/>
-      <c r="I195" s="7"/>
-    </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I195" s="9"/>
+      <c r="J195" s="7"/>
+    </row>
+    <row r="196" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A196" s="8"/>
       <c r="B196" s="9"/>
       <c r="C196" s="9"/>
@@ -3477,9 +3708,10 @@
       <c r="F196" s="9"/>
       <c r="G196" s="9"/>
       <c r="H196" s="9"/>
-      <c r="I196" s="7"/>
-    </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I196" s="9"/>
+      <c r="J196" s="7"/>
+    </row>
+    <row r="197" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A197" s="8"/>
       <c r="B197" s="9"/>
       <c r="C197" s="9"/>
@@ -3488,9 +3720,10 @@
       <c r="F197" s="9"/>
       <c r="G197" s="9"/>
       <c r="H197" s="9"/>
-      <c r="I197" s="7"/>
-    </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I197" s="9"/>
+      <c r="J197" s="7"/>
+    </row>
+    <row r="198" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A198" s="8"/>
       <c r="B198" s="9"/>
       <c r="C198" s="9"/>
@@ -3499,9 +3732,10 @@
       <c r="F198" s="9"/>
       <c r="G198" s="9"/>
       <c r="H198" s="9"/>
-      <c r="I198" s="7"/>
-    </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I198" s="9"/>
+      <c r="J198" s="7"/>
+    </row>
+    <row r="199" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A199" s="8"/>
       <c r="B199" s="9"/>
       <c r="C199" s="9"/>
@@ -3510,9 +3744,10 @@
       <c r="F199" s="9"/>
       <c r="G199" s="9"/>
       <c r="H199" s="9"/>
-      <c r="I199" s="7"/>
-    </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I199" s="9"/>
+      <c r="J199" s="7"/>
+    </row>
+    <row r="200" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A200" s="8"/>
       <c r="B200" s="9"/>
       <c r="C200" s="9"/>
@@ -3521,9 +3756,10 @@
       <c r="F200" s="9"/>
       <c r="G200" s="9"/>
       <c r="H200" s="9"/>
-      <c r="I200" s="7"/>
-    </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I200" s="9"/>
+      <c r="J200" s="7"/>
+    </row>
+    <row r="201" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A201" s="10"/>
       <c r="B201" s="11"/>
       <c r="C201" s="11"/>
@@ -3532,7 +3768,8 @@
       <c r="F201" s="11"/>
       <c r="G201" s="11"/>
       <c r="H201" s="11"/>
-      <c r="I201" s="12"/>
+      <c r="I201" s="11"/>
+      <c r="J201" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Restrict data caching for entities not associated with OUs/Folders
</commit_message>
<xml_diff>
--- a/Workbooks/EN/Processes.xlsx
+++ b/Workbooks/EN/Processes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Workbooks\EN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A8031F9-52E1-4457-9FC2-2011D2581EAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA492F6-4C40-491D-9174-F46BA7FDE322}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3945,8 +3945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G201"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>